<commit_message>
some columns were translated
</commit_message>
<xml_diff>
--- a/santander-customer-satisfaction/documents/columns_rename.xlsx
+++ b/santander-customer-satisfaction/documents/columns_rename.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Git\Santander\EVS_KAGGLE_TEAM\santander-customer-satisfaction\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8EC15A2-234A-4B99-AEE9-F879FEE1F6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0093986E-EEC6-4DB8-A1F2-49F27B7CDF52}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="573">
   <si>
     <t>original_cols</t>
   </si>
@@ -1675,12 +1674,81 @@
   </si>
   <si>
     <t>delta_sales_fee_var44_1&amp;3</t>
+  </si>
+  <si>
+    <t>delta_num_dep_var13_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_dep_var17_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_dep_var33_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_buy_var44_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_reimb_var13_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_reimb_var17_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_reimb_var33_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_transf_var17_in_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_transf_var17_out_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_transf_var33_in_1y3</t>
+  </si>
+  <si>
+    <t>delta_num_transf_var33_out_1y3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var18_last3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var34_last3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var13_last3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var17_last3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var33_last3</t>
+  </si>
+  <si>
+    <t>redemption_amount_var18_last1</t>
+  </si>
+  <si>
+    <t>redemption_amount_var13_last1</t>
+  </si>
+  <si>
+    <t>redemption_amount_var17_last1</t>
+  </si>
+  <si>
+    <t>redemption_amount_var34_last1</t>
+  </si>
+  <si>
+    <t>redemption_amount_var33_last1</t>
+  </si>
+  <si>
+    <t>buy_amount_var44_last3</t>
+  </si>
+  <si>
+    <t>buy_amount_var44_last1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1734,14 +1802,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0185E1A-5210-4177-AB00-33407698672F}" name="Table1" displayName="Table1" ref="A1:B372" totalsRowShown="0">
-  <autoFilter ref="A1:B372" xr:uid="{F0185E1A-5210-4177-AB00-33407698672F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B372">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B372" totalsRowShown="0">
+  <autoFilter ref="A1:B372"/>
+  <sortState ref="A2:B372">
     <sortCondition ref="A1:A372"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{65281D84-D624-4F5E-9D00-77A1E2D045CC}" name="original_cols"/>
-    <tableColumn id="2" xr3:uid="{BC0CF87A-C533-47B1-B289-AC5F4C95B5A1}" name="new_name"/>
+    <tableColumn id="1" name="original_cols"/>
+    <tableColumn id="2" name="new_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2043,20 +2111,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0172C4-BD31-4FCF-96F1-0156E80224B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L372"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2064,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2072,7 +2140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +2148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2088,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2103,7 +2171,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2186,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2133,7 +2201,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2216,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2163,7 +2231,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2178,7 +2246,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2193,7 +2261,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2208,7 +2276,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2223,7 +2291,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2238,7 +2306,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2253,9 +2321,12 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>550</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
@@ -2265,9 +2336,12 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>551</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2277,9 +2351,12 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>552</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2289,9 +2366,12 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>553</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2301,9 +2381,12 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>554</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2313,9 +2396,12 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>555</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2325,9 +2411,12 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>556</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2337,9 +2426,12 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>557</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
@@ -2349,9 +2441,12 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>558</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2361,9 +2456,12 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>559</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2373,9 +2471,12 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>560</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2385,7 +2486,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2400,8 +2501,11 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
       </c>
       <c r="F28" s="1"/>
@@ -2412,9 +2516,12 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>561</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
@@ -2424,9 +2531,12 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>566</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2436,9 +2546,12 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>562</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2448,9 +2561,12 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>569</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2460,9 +2576,12 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>563</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2472,9 +2591,12 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>567</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2484,9 +2606,12 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>564</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2496,32 +2621,47 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2529,7 +2669,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2537,7 +2677,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2545,102 +2685,102 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -2648,77 +2788,77 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>95</v>
       </c>
@@ -2726,7 +2866,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -2734,7 +2874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -2742,7 +2882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>101</v>
       </c>
@@ -2750,7 +2890,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>103</v>
       </c>
@@ -2758,7 +2898,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>105</v>
       </c>
@@ -2766,7 +2906,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>107</v>
       </c>
@@ -2774,7 +2914,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -2782,7 +2922,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>111</v>
       </c>
@@ -2790,7 +2930,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -2798,7 +2938,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>115</v>
       </c>
@@ -2806,7 +2946,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>117</v>
       </c>
@@ -2814,7 +2954,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -2822,7 +2962,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -2830,7 +2970,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>123</v>
       </c>
@@ -2838,7 +2978,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>125</v>
       </c>
@@ -2846,7 +2986,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>127</v>
       </c>
@@ -2854,7 +2994,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>129</v>
       </c>
@@ -2862,7 +3002,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>131</v>
       </c>
@@ -2870,7 +3010,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>133</v>
       </c>
@@ -2878,7 +3018,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>135</v>
       </c>
@@ -2886,7 +3026,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>137</v>
       </c>
@@ -2894,7 +3034,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -2902,7 +3042,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -2910,7 +3050,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>143</v>
       </c>
@@ -2918,7 +3058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>145</v>
       </c>
@@ -2926,7 +3066,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>147</v>
       </c>
@@ -2934,7 +3074,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>149</v>
       </c>
@@ -2942,7 +3082,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>151</v>
       </c>
@@ -2950,7 +3090,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>153</v>
       </c>
@@ -2958,7 +3098,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>155</v>
       </c>
@@ -2966,7 +3106,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>157</v>
       </c>
@@ -2974,7 +3114,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>159</v>
       </c>
@@ -2982,7 +3122,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>161</v>
       </c>
@@ -2990,7 +3130,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>163</v>
       </c>
@@ -2998,7 +3138,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>165</v>
       </c>
@@ -3006,7 +3146,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>167</v>
       </c>
@@ -3014,7 +3154,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>169</v>
       </c>
@@ -3022,7 +3162,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>171</v>
       </c>
@@ -3030,7 +3170,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>173</v>
       </c>
@@ -3038,7 +3178,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>175</v>
       </c>
@@ -3046,7 +3186,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>177</v>
       </c>
@@ -3054,7 +3194,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>179</v>
       </c>
@@ -3062,7 +3202,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>181</v>
       </c>
@@ -3070,7 +3210,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>183</v>
       </c>
@@ -3078,7 +3218,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>185</v>
       </c>
@@ -3086,7 +3226,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>187</v>
       </c>
@@ -3094,7 +3234,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>189</v>
       </c>
@@ -3102,7 +3242,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>191</v>
       </c>
@@ -3110,7 +3250,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>193</v>
       </c>
@@ -3118,7 +3258,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>195</v>
       </c>
@@ -3126,7 +3266,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>197</v>
       </c>
@@ -3134,7 +3274,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>199</v>
       </c>
@@ -3142,7 +3282,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>201</v>
       </c>
@@ -3150,7 +3290,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>203</v>
       </c>
@@ -3158,7 +3298,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>205</v>
       </c>
@@ -3166,7 +3306,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>207</v>
       </c>
@@ -3174,7 +3314,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>209</v>
       </c>
@@ -3182,7 +3322,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>211</v>
       </c>
@@ -3190,7 +3330,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>213</v>
       </c>
@@ -3198,7 +3338,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>215</v>
       </c>
@@ -3206,7 +3346,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>217</v>
       </c>
@@ -3214,7 +3354,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>219</v>
       </c>
@@ -3222,7 +3362,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>221</v>
       </c>
@@ -3230,7 +3370,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>223</v>
       </c>
@@ -3238,7 +3378,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>225</v>
       </c>
@@ -3246,7 +3386,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>227</v>
       </c>
@@ -3254,7 +3394,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>229</v>
       </c>
@@ -3262,7 +3402,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>231</v>
       </c>
@@ -3270,82 +3410,82 @@
         <v>232</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>248</v>
       </c>
@@ -3353,7 +3493,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>250</v>
       </c>
@@ -3361,7 +3501,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>252</v>
       </c>
@@ -3369,7 +3509,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>254</v>
       </c>
@@ -3377,7 +3517,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>256</v>
       </c>
@@ -3385,7 +3525,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>258</v>
       </c>
@@ -3393,7 +3533,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>260</v>
       </c>
@@ -3401,7 +3541,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>262</v>
       </c>
@@ -3409,7 +3549,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>264</v>
       </c>
@@ -3417,12 +3557,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>267</v>
       </c>
@@ -3430,7 +3570,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>269</v>
       </c>
@@ -3438,7 +3578,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>271</v>
       </c>
@@ -3446,317 +3586,317 @@
         <v>272</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>335</v>
       </c>
@@ -3764,7 +3904,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>337</v>
       </c>
@@ -3772,292 +3912,292 @@
         <v>338</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>396</v>
       </c>
@@ -4065,7 +4205,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>398</v>
       </c>
@@ -4073,7 +4213,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>400</v>
       </c>
@@ -4081,7 +4221,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>402</v>
       </c>
@@ -4089,7 +4229,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>404</v>
       </c>
@@ -4097,7 +4237,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>406</v>
       </c>
@@ -4105,7 +4245,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>408</v>
       </c>
@@ -4113,7 +4253,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>410</v>
       </c>
@@ -4121,7 +4261,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>412</v>
       </c>
@@ -4129,7 +4269,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>414</v>
       </c>
@@ -4137,7 +4277,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>416</v>
       </c>
@@ -4145,7 +4285,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>418</v>
       </c>
@@ -4153,7 +4293,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>420</v>
       </c>
@@ -4161,7 +4301,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>422</v>
       </c>
@@ -4169,7 +4309,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>424</v>
       </c>
@@ -4177,7 +4317,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>426</v>
       </c>
@@ -4185,7 +4325,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>428</v>
       </c>
@@ -4193,7 +4333,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>430</v>
       </c>
@@ -4201,7 +4341,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>432</v>
       </c>
@@ -4209,7 +4349,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>434</v>
       </c>
@@ -4217,7 +4357,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>436</v>
       </c>
@@ -4225,7 +4365,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>438</v>
       </c>
@@ -4233,7 +4373,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>440</v>
       </c>
@@ -4241,7 +4381,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>442</v>
       </c>
@@ -4249,7 +4389,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>444</v>
       </c>
@@ -4257,7 +4397,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>446</v>
       </c>
@@ -4265,7 +4405,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>448</v>
       </c>
@@ -4273,7 +4413,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>450</v>
       </c>
@@ -4281,7 +4421,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>452</v>
       </c>
@@ -4289,7 +4429,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>454</v>
       </c>
@@ -4297,7 +4437,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>456</v>
       </c>
@@ -4305,7 +4445,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>458</v>
       </c>
@@ -4313,7 +4453,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>460</v>
       </c>
@@ -4321,7 +4461,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>462</v>
       </c>
@@ -4329,7 +4469,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>464</v>
       </c>
@@ -4337,7 +4477,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>466</v>
       </c>
@@ -4345,7 +4485,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>468</v>
       </c>
@@ -4353,7 +4493,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>470</v>
       </c>
@@ -4361,7 +4501,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>472</v>
       </c>
@@ -4369,7 +4509,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>474</v>
       </c>
@@ -4377,7 +4517,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>476</v>
       </c>
@@ -4385,7 +4525,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>478</v>
       </c>
@@ -4393,7 +4533,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>480</v>
       </c>
@@ -4401,7 +4541,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>482</v>
       </c>
@@ -4409,7 +4549,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>484</v>
       </c>
@@ -4417,7 +4557,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>486</v>
       </c>
@@ -4425,7 +4565,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>488</v>
       </c>
@@ -4433,7 +4573,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>490</v>
       </c>
@@ -4441,7 +4581,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>492</v>
       </c>
@@ -4449,7 +4589,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>494</v>
       </c>
@@ -4457,7 +4597,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>496</v>
       </c>
@@ -4465,7 +4605,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>498</v>
       </c>
@@ -4473,7 +4613,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>500</v>
       </c>
@@ -4481,7 +4621,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>502</v>
       </c>
@@ -4489,7 +4629,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>504</v>
       </c>
@@ -4497,7 +4637,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>506</v>
       </c>
@@ -4505,7 +4645,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>508</v>
       </c>
@@ -4513,7 +4653,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>510</v>
       </c>
@@ -4521,7 +4661,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>512</v>
       </c>
@@ -4529,7 +4669,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>514</v>
       </c>
@@ -4537,7 +4677,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>516</v>
       </c>
@@ -4545,7 +4685,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>518</v>
       </c>
@@ -4553,7 +4693,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>520</v>
       </c>
@@ -4561,7 +4701,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>522</v>
       </c>
@@ -4569,7 +4709,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>524</v>
       </c>
@@ -4577,7 +4717,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>526</v>
       </c>
@@ -4585,7 +4725,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>528</v>
       </c>
@@ -4593,7 +4733,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>530</v>
       </c>
@@ -4601,7 +4741,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>532</v>
       </c>
@@ -4609,7 +4749,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>534</v>
       </c>
@@ -4617,7 +4757,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>536</v>
       </c>
@@ -4625,12 +4765,12 @@
         <v>537</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>539</v>
       </c>
@@ -4638,7 +4778,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>541</v>
       </c>
@@ -4646,7 +4786,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>543</v>
       </c>
@@ -4654,7 +4794,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>545</v>
       </c>
@@ -4662,7 +4802,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>547</v>
       </c>

</xml_diff>